<commit_message>
Added tables after the displayed image was re-orientated. Added more conclusions
</commit_message>
<xml_diff>
--- a/QR_codes/Vetscan_QR_label_Docs/QR_code_results_chart.xlsx
+++ b/QR_codes/Vetscan_QR_label_Docs/QR_code_results_chart.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GRAHAMB\Documents\Camera\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Zoetis\QR_codes\Vetscan_QR_label_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ACCED7-90EC-4A6A-9061-69F9CEA9D5EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1B2472-AFA3-4BC6-A5B6-3264777D65CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="manual" sheetId="1" r:id="rId1"/>
     <sheet name="auto.vs.fixed" sheetId="2" r:id="rId2"/>
+    <sheet name="auto.vs.fixed.rotated" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <r>
       <t>10</t>
@@ -85,6 +86,36 @@
   </si>
   <si>
     <t>autofocus averages</t>
+  </si>
+  <si>
+    <t>mm x mm</t>
+  </si>
+  <si>
+    <t>10x10</t>
+  </si>
+  <si>
+    <t>20x20</t>
+  </si>
+  <si>
+    <t>50x50</t>
+  </si>
+  <si>
+    <t>10x10 Bruce</t>
+  </si>
+  <si>
+    <t>10x10 Brian</t>
+  </si>
+  <si>
+    <t>20x20 Bruce</t>
+  </si>
+  <si>
+    <t>20x20 Brian</t>
+  </si>
+  <si>
+    <t>50x50 Bruce</t>
+  </si>
+  <si>
+    <t>50x50 Brain</t>
   </si>
 </sst>
 </file>
@@ -215,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -251,6 +282,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,9 +1053,35 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'auto.vs.fixed'!$F$3:$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10x10 Bruce</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10x10 Brian</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20x20 Bruce</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20x20 Brian</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50x50 Bruce</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50x50 Brain</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'auto.vs.fixed'!$F$3:$F$8</c:f>
+              <c:f>'auto.vs.fixed'!$G$3:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1054,7 +1118,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'auto.vs.fixed'!$G$2</c:f>
+              <c:f>'auto.vs.fixed'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1075,9 +1139,35 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'auto.vs.fixed'!$F$3:$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10x10 Bruce</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10x10 Brian</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20x20 Bruce</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20x20 Brian</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50x50 Bruce</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50x50 Brain</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'auto.vs.fixed'!$G$3:$G$8</c:f>
+              <c:f>'auto.vs.fixed'!$H$3:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1128,6 +1218,382 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="528158664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="528158664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="528156040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Blue:</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> autofocus  Orange: fixed focus</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'auto.vs.fixed.rotated'!$F$3:$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10x10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20x20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50x50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'auto.vs.fixed.rotated'!$G$3:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.4899999999999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1130-44CA-8D5A-CC937C23FAB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'auto.vs.fixed.rotated'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fixed focus averages</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'auto.vs.fixed.rotated'!$F$3:$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10x10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20x20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50x50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'auto.vs.fixed.rotated'!$H$3:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2475000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.085000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1130-44CA-8D5A-CC937C23FAB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="528156040"/>
+        <c:axId val="528158664"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="528156040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1359,6 +1825,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1876,6 +2382,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2436,13 +3458,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
@@ -2457,6 +3479,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{405B30BF-2D55-4C78-856D-999FB6752620}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2776,12 +3841,12 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" customWidth="1"/>
+    <col min="1" max="1" width="38.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2792,7 +3857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -2806,7 +3871,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2820,7 +3885,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -2834,7 +3899,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -2848,7 +3913,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -2862,7 +3927,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
@@ -2876,8 +3941,8 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="7">
         <v>0</v>
       </c>
@@ -2888,7 +3953,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="5">
         <v>450</v>
       </c>
@@ -2899,7 +3964,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="5">
         <v>0</v>
       </c>
@@ -2910,7 +3975,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="5">
         <v>0</v>
       </c>
@@ -2921,7 +3986,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="5">
         <v>152</v>
       </c>
@@ -2932,7 +3997,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="9">
         <v>122</v>
       </c>
@@ -2952,126 +4017,148 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A07BF2-8A8D-4E54-8745-2251B92405B3}">
-  <dimension ref="B2:G29"/>
+  <dimension ref="B2:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="6" max="6" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" s="11" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" s="11" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="9">
         <v>4.87</v>
       </c>
       <c r="D3" s="9">
         <v>2.58</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="10">
         <f>AVERAGE(B3:B5)</f>
         <v>7.38</v>
       </c>
-      <c r="G3" s="10">
+      <c r="H3" s="10">
         <f>AVERAGE(D3:D5)</f>
         <v>2.69</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="5">
         <v>7.63</v>
       </c>
       <c r="D4" s="5">
         <v>2.35</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="10">
         <f>AVERAGE(B7:B9)</f>
         <v>5.8633333333333333</v>
       </c>
-      <c r="G4" s="10">
+      <c r="H4" s="10">
         <f>AVERAGE(D7:D9)</f>
         <v>3.7399999999999998</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="5">
         <v>9.64</v>
       </c>
       <c r="D5" s="5">
         <v>3.14</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="10">
         <f>AVERAGE(B11:B14)</f>
         <v>3.69</v>
       </c>
-      <c r="G5" s="10">
+      <c r="H5" s="10">
         <f>AVERAGE(D11:D14)</f>
         <v>3.0300000000000002</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="F6" s="10">
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="10">
         <f>AVERAGE(B16:B19)</f>
         <v>6.2675000000000001</v>
       </c>
-      <c r="G6" s="10">
+      <c r="H6" s="10">
         <f>AVERAGE(D16:D19)</f>
         <v>2.6375000000000002</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="5">
         <v>5.71</v>
       </c>
       <c r="D7" s="5">
         <v>2.63</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="10">
         <f>AVERAGE(B21:B24)</f>
         <v>14.52</v>
       </c>
-      <c r="G7" s="10">
+      <c r="H7" s="10">
         <f>AVERAGE(D21:D24)</f>
         <v>7.23</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="5">
         <v>6.05</v>
       </c>
       <c r="D8" s="5">
         <v>3.12</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="10">
         <f>AVERAGE(B26:B29)</f>
         <v>4.33</v>
       </c>
-      <c r="G8" s="10">
+      <c r="H8" s="10">
         <f>AVERAGE(D26:D29)</f>
         <v>6.51</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="5">
         <v>5.83</v>
       </c>
@@ -3079,11 +4166,11 @@
         <v>5.47</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="5"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5">
         <v>4.13</v>
       </c>
@@ -3091,7 +4178,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="5">
         <v>3.17</v>
       </c>
@@ -3099,7 +4186,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="5">
         <v>3.88</v>
       </c>
@@ -3107,7 +4194,7 @@
         <v>5.58</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="5">
         <v>3.58</v>
       </c>
@@ -3115,11 +4202,11 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="5"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="5">
         <v>4.26</v>
       </c>
@@ -3127,7 +4214,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="5">
         <v>6.37</v>
       </c>
@@ -3135,7 +4222,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="5">
         <v>9.4600000000000009</v>
       </c>
@@ -3143,7 +4230,7 @@
         <v>2.54</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="5">
         <v>4.9800000000000004</v>
       </c>
@@ -3151,11 +4238,11 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="5"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="5">
         <v>8.34</v>
       </c>
@@ -3163,7 +4250,7 @@
         <v>6.09</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="5">
         <v>15.98</v>
       </c>
@@ -3171,7 +4258,7 @@
         <v>6.74</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="5">
         <v>18.03</v>
       </c>
@@ -3179,7 +4266,7 @@
         <v>7.09</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="5">
         <v>15.73</v>
       </c>
@@ -3187,11 +4274,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="5"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="5">
         <v>4.08</v>
       </c>
@@ -3199,7 +4286,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="5">
         <v>4.37</v>
       </c>
@@ -3207,7 +4294,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="5">
         <v>3.85</v>
       </c>
@@ -3215,13 +4302,278 @@
         <v>8.2899999999999991</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="5">
         <v>5.0199999999999996</v>
       </c>
       <c r="D29" s="5">
         <v>9.7200000000000006</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0ED1C1-28BD-4D3F-A077-8CF8F8E1B7B9}">
+  <dimension ref="B2:H29"/>
+  <sheetViews>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="11.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" s="11" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="9">
+        <v>6.53</v>
+      </c>
+      <c r="D3" s="9">
+        <v>2.33</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="10">
+        <f>AVERAGE(B3:B5)</f>
+        <v>6.4899999999999993</v>
+      </c>
+      <c r="H3" s="10">
+        <f>AVERAGE(D3:D5)</f>
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="5">
+        <v>5.05</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3.52</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="10">
+        <f>AVERAGE(B7:B10)</f>
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="H4" s="10">
+        <f>AVERAGE(D7:D10)</f>
+        <v>3.2475000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="5">
+        <v>7.89</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="10">
+        <f>AVERAGE(B12:B14)</f>
+        <v>7.78</v>
+      </c>
+      <c r="H5" s="10">
+        <f>AVERAGE(D12:D15)</f>
+        <v>11.085000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="5">
+        <v>3.73</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="5">
+        <v>11.77</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3.72</v>
+      </c>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="5">
+        <v>8.93</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2.69</v>
+      </c>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="5">
+        <v>8.69</v>
+      </c>
+      <c r="D10" s="5">
+        <v>4.34</v>
+      </c>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="5">
+        <v>5.16</v>
+      </c>
+      <c r="D12" s="5">
+        <v>6.17</v>
+      </c>
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="5">
+        <v>12.41</v>
+      </c>
+      <c r="D13" s="5">
+        <v>7.22</v>
+      </c>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="13">
+        <v>5.77</v>
+      </c>
+      <c r="D14" s="5">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="5">
+        <v>13.96</v>
+      </c>
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added results of using a darker diffuser.
</commit_message>
<xml_diff>
--- a/QR_codes/Vetscan_QR_label_Docs/QR_code_results_chart.xlsx
+++ b/QR_codes/Vetscan_QR_label_Docs/QR_code_results_chart.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Zoetis\QR_codes\Vetscan_QR_label_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1B2472-AFA3-4BC6-A5B6-3264777D65CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA415172-2BD1-499A-A9F5-77744BA9B1D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="manual" sheetId="1" r:id="rId1"/>
     <sheet name="auto.vs.fixed" sheetId="2" r:id="rId2"/>
     <sheet name="auto.vs.fixed.rotated" sheetId="3" r:id="rId3"/>
+    <sheet name="diffuser#2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <r>
       <t>10</t>
@@ -117,6 +118,24 @@
   <si>
     <t>50x50 Brain</t>
   </si>
+  <si>
+    <t>QR Version</t>
+  </si>
+  <si>
+    <t>10 x 10</t>
+  </si>
+  <si>
+    <t>20 x 20</t>
+  </si>
+  <si>
+    <t>50 x 50</t>
+  </si>
+  <si>
+    <t>diffuser#1 autofocus</t>
+  </si>
+  <si>
+    <t>diffuser#2 autofocus</t>
+  </si>
 </sst>
 </file>
 
@@ -157,7 +176,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,8 +189,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -242,11 +267,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -289,6 +329,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1745,6 +1794,384 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Blue:</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> diffuser#1  Orange: diffuser#2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>diffuser#1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'diffuser#2'!$C$4:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.89</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.93</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.41</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6CAB-48CA-B1C8-909A60A33946}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>diffuser#2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'diffuser#2'!$D$4:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.79</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.3099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.51</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-6CAB-48CA-B1C8-909A60A33946}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="528156040"/>
+        <c:axId val="528158664"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="528156040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="528158664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="528158664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="528156040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1865,6 +2292,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2898,6 +3365,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3516,6 +4499,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{405B30BF-2D55-4C78-856D-999FB6752620}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDF679B7-2DE0-452F-9CA2-5B84B0621465}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3841,12 +4867,12 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.81640625" customWidth="1"/>
+    <col min="1" max="1" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3857,7 +4883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -3871,7 +4897,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -3885,7 +4911,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -3899,7 +4925,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -3913,7 +4939,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -3927,7 +4953,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
@@ -3941,8 +4967,8 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>0</v>
       </c>
@@ -3953,7 +4979,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
         <v>450</v>
       </c>
@@ -3964,7 +4990,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
         <v>0</v>
       </c>
@@ -3975,7 +5001,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5">
         <v>0</v>
       </c>
@@ -3986,7 +5012,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
         <v>152</v>
       </c>
@@ -3997,7 +5023,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="9">
         <v>122</v>
       </c>
@@ -4019,19 +5045,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A07BF2-8A8D-4E54-8745-2251B92405B3}">
   <dimension ref="B2:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" s="11" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:8" s="11" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
@@ -4048,7 +5074,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9">
         <v>4.87</v>
       </c>
@@ -4067,7 +5093,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>7.63</v>
       </c>
@@ -4086,7 +5112,7 @@
         <v>3.7399999999999998</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5">
         <v>9.64</v>
       </c>
@@ -4105,7 +5131,7 @@
         <v>3.0300000000000002</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="D6" s="5"/>
       <c r="F6" t="s">
@@ -4120,7 +5146,7 @@
         <v>2.6375000000000002</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>5.71</v>
       </c>
@@ -4139,7 +5165,7 @@
         <v>7.23</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
         <v>6.05</v>
       </c>
@@ -4158,7 +5184,7 @@
         <v>6.51</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>5.83</v>
       </c>
@@ -4166,11 +5192,11 @@
         <v>5.47</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <v>4.13</v>
       </c>
@@ -4178,7 +5204,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5">
         <v>3.17</v>
       </c>
@@ -4186,7 +5212,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>3.88</v>
       </c>
@@ -4194,7 +5220,7 @@
         <v>5.58</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
         <v>3.58</v>
       </c>
@@ -4202,11 +5228,11 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
         <v>4.26</v>
       </c>
@@ -4214,7 +5240,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5">
         <v>6.37</v>
       </c>
@@ -4222,7 +5248,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
         <v>9.4600000000000009</v>
       </c>
@@ -4230,7 +5256,7 @@
         <v>2.54</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="5">
         <v>4.9800000000000004</v>
       </c>
@@ -4238,11 +5264,11 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="5">
         <v>8.34</v>
       </c>
@@ -4250,7 +5276,7 @@
         <v>6.09</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="5">
         <v>15.98</v>
       </c>
@@ -4258,7 +5284,7 @@
         <v>6.74</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5">
         <v>18.03</v>
       </c>
@@ -4266,7 +5292,7 @@
         <v>7.09</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="5">
         <v>15.73</v>
       </c>
@@ -4274,11 +5300,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5">
         <v>4.08</v>
       </c>
@@ -4286,7 +5312,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="5">
         <v>4.37</v>
       </c>
@@ -4294,7 +5320,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="5">
         <v>3.85</v>
       </c>
@@ -4302,7 +5328,7 @@
         <v>8.2899999999999991</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5">
         <v>5.0199999999999996</v>
       </c>
@@ -4322,17 +5348,17 @@
   <dimension ref="B2:H29"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" s="11" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:8" s="11" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
@@ -4350,7 +5376,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9">
         <v>6.53</v>
       </c>
@@ -4370,7 +5396,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>5.05</v>
       </c>
@@ -4390,7 +5416,7 @@
         <v>3.2475000000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5">
         <v>7.89</v>
       </c>
@@ -4410,12 +5436,12 @@
         <v>11.085000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>3.73</v>
       </c>
@@ -4424,7 +5450,7 @@
       </c>
       <c r="E7" s="14"/>
     </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
         <v>11.77</v>
       </c>
@@ -4433,7 +5459,7 @@
       </c>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>8.93</v>
       </c>
@@ -4442,7 +5468,7 @@
       </c>
       <c r="E9" s="14"/>
     </row>
-    <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
         <v>8.69</v>
       </c>
@@ -4451,12 +5477,12 @@
       </c>
       <c r="E10" s="14"/>
     </row>
-    <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5">
         <v>5.16</v>
       </c>
@@ -4465,7 +5491,7 @@
       </c>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>12.41</v>
       </c>
@@ -4474,7 +5500,7 @@
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="13">
         <v>5.77</v>
       </c>
@@ -4483,7 +5509,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
       <c r="D15" s="5">
@@ -4491,89 +5517,285 @@
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="15"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
       <c r="C20" s="15"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1856A8E-6C1C-4ADD-B10A-8037C48A3222}">
+  <dimension ref="A2:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="16"/>
+      <c r="D2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>5</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="18">
+        <v>6.53</v>
+      </c>
+      <c r="D4" s="18">
+        <v>10.79</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>6</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="18">
+        <v>5.05</v>
+      </c>
+      <c r="D5" s="18">
+        <v>11.89</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <v>7</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="18">
+        <v>7.89</v>
+      </c>
+      <c r="D6" s="18">
+        <v>8.48</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
+        <v>14</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="18">
+        <v>3.73</v>
+      </c>
+      <c r="D7" s="18">
+        <v>5.67</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
+        <v>15</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="18">
+        <v>11.77</v>
+      </c>
+      <c r="D8" s="18">
+        <v>5.73</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <v>16</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="18">
+        <v>8.93</v>
+      </c>
+      <c r="D9" s="18">
+        <v>8.51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
+        <v>17</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="18">
+        <v>8.69</v>
+      </c>
+      <c r="D10" s="18">
+        <v>4.3099999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
+        <v>26</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="18">
+        <v>5.16</v>
+      </c>
+      <c r="D11" s="18">
+        <v>3.64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
+        <v>27</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="18">
+        <v>12.41</v>
+      </c>
+      <c r="D12" s="18">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <v>29</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="18">
+        <v>5.77</v>
+      </c>
+      <c r="D13" s="18">
+        <v>3.59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
camera image rotate, not flip
</commit_message>
<xml_diff>
--- a/QR_codes/Vetscan_QR_label_Docs/QR_code_results_chart.xlsx
+++ b/QR_codes/Vetscan_QR_label_Docs/QR_code_results_chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Zoetis\QR_codes\Vetscan_QR_label_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA415172-2BD1-499A-A9F5-77744BA9B1D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C874DCBE-0620-4152-B09C-CCD38C28AA0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1836,6 +1836,24 @@
               <a:t> diffuser#1  Orange: diffuser#2</a:t>
             </a:r>
           </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Blue dots: trend diffuser#1</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Orange dots: trend diffuse#2</a:t>
+            </a:r>
+          </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
@@ -1891,6 +1909,20 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:val>
             <c:numRef>
               <c:f>'diffuser#2'!$C$4:$C$13</c:f>
@@ -1955,6 +1987,20 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:val>
             <c:numRef>
               <c:f>'diffuser#2'!$D$4:$D$13</c:f>
@@ -4526,15 +4572,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5613,7 +5659,7 @@
   <dimension ref="A2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Experiments and test results with diffusers.
</commit_message>
<xml_diff>
--- a/QR_codes/Vetscan_QR_label_Docs/QR_code_results_chart.xlsx
+++ b/QR_codes/Vetscan_QR_label_Docs/QR_code_results_chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Zoetis\QR_codes\Vetscan_QR_label_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C874DCBE-0620-4152-B09C-CCD38C28AA0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DCDB25-4B04-48B8-81A0-7544E411D393}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-516" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="manual" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <r>
       <t>10</t>
@@ -176,7 +176,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,8 +195,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -282,11 +288,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -332,10 +351,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1851,7 +1882,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Orange dots: trend diffuse#2</a:t>
+              <a:t>Orange dots: trend diffuser#2 (less glare)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1923,41 +1954,122 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'diffuser#2'!$A$4:$B$14</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="11"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>10 x 10</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10 x 10</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>10 x 10</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>20 x 20</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>20 x 20</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>20 x 20</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>20 x 20</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>50 x 50</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>50 x 50</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>50 x 50</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>50 x 50</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>14</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>17</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>17</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>18</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'diffuser#2'!$C$4:$C$13</c:f>
+              <c:f>'diffuser#2'!$C$4:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>6.53</c:v>
+                  <c:v>4.87</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.05</c:v>
+                  <c:v>7.63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.89</c:v>
+                  <c:v>9.64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.73</c:v>
+                  <c:v>4.13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.77</c:v>
+                  <c:v>3.17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.93</c:v>
+                  <c:v>3.88</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.69</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.16</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12.41</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.77</c:v>
+                  <c:v>3.58</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00">
+                  <c:v>6.09</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00">
+                  <c:v>6.74</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00">
+                  <c:v>7.09</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00">
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2001,40 +2113,121 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'diffuser#2'!$A$4:$B$14</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="11"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>10 x 10</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10 x 10</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>10 x 10</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>20 x 20</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>20 x 20</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>20 x 20</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>20 x 20</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>50 x 50</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>50 x 50</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>50 x 50</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>50 x 50</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>14</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>17</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>17</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>18</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'diffuser#2'!$D$4:$D$13</c:f>
+              <c:f>'diffuser#2'!$D$4:$D$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>4.9400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10.79</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.89</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.48</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>5.67</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5.73</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>8.51</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>4.3099999999999996</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>3.64</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>4.51</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>3.59</c:v>
                 </c:pt>
               </c:numCache>
@@ -2143,7 +2336,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="180000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -4571,8 +4764,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
@@ -5092,7 +5285,7 @@
   <dimension ref="B2:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5394,7 +5587,7 @@
   <dimension ref="B2:H29"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5656,10 +5849,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1856A8E-6C1C-4ADD-B10A-8037C48A3222}">
-  <dimension ref="A2:H13"/>
+  <dimension ref="A2:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5678,168 +5871,182 @@
       <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="22" t="s">
         <v>28</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>5</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="18">
-        <v>6.53</v>
+      <c r="C4" s="17">
+        <v>4.87</v>
       </c>
       <c r="D4" s="18">
-        <v>10.79</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
+      <c r="A5" s="17">
         <v>6</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="18">
-        <v>5.05</v>
-      </c>
-      <c r="D5" s="18">
-        <v>11.89</v>
+      <c r="C5" s="17">
+        <v>7.63</v>
+      </c>
+      <c r="D5" s="19">
+        <v>4.53</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+      <c r="A6" s="17">
         <v>7</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="18">
-        <v>7.89</v>
-      </c>
-      <c r="D6" s="18">
-        <v>8.48</v>
+      <c r="C6" s="17">
+        <v>9.64</v>
+      </c>
+      <c r="D6" s="19">
+        <v>10.79</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="A7" s="17">
         <v>14</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="18">
-        <v>3.73</v>
-      </c>
-      <c r="D7" s="18">
-        <v>5.67</v>
+      <c r="C7" s="17">
+        <v>4.13</v>
+      </c>
+      <c r="D7" s="19">
+        <v>8.48</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
+      <c r="A8" s="17">
         <v>15</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="18">
-        <v>11.77</v>
-      </c>
-      <c r="D8" s="18">
-        <v>5.73</v>
+      <c r="C8" s="17">
+        <v>3.17</v>
+      </c>
+      <c r="D8" s="19">
+        <v>5.67</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+      <c r="A9" s="17">
         <v>16</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="18">
-        <v>8.93</v>
-      </c>
-      <c r="D9" s="18">
+      <c r="C9" s="17">
+        <v>3.88</v>
+      </c>
+      <c r="D9" s="19">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>17</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="17">
+        <v>3.58</v>
+      </c>
+      <c r="D10" s="19">
         <v>8.51</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>15</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="19">
+        <v>6.09</v>
+      </c>
+      <c r="D11" s="19">
+        <v>4.3099999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
+        <v>16</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="19">
+        <v>6.74</v>
+      </c>
+      <c r="D12" s="19">
+        <v>3.64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
         <v>17</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="18">
-        <v>8.69</v>
-      </c>
-      <c r="D10" s="18">
-        <v>4.3099999999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
+      <c r="B13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="C13" s="19">
+        <v>7.09</v>
+      </c>
+      <c r="D13" s="19">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>18</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="18">
-        <v>5.16</v>
-      </c>
-      <c r="D11" s="18">
-        <v>3.64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
-        <v>27</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="18">
-        <v>12.41</v>
-      </c>
-      <c r="D12" s="18">
-        <v>4.51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
-        <v>29</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="18">
-        <v>5.77</v>
-      </c>
-      <c r="D13" s="18">
+      <c r="C14" s="19">
+        <v>9</v>
+      </c>
+      <c r="D14" s="19">
         <v>3.59</v>
       </c>
     </row>

</xml_diff>